<commit_message>
update growth rate equation and bleeding ratio in template
</commit_message>
<xml_diff>
--- a/input_files/perfusion_data.xlsx
+++ b/input_files/perfusion_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galileo/development/Reserch/UMN_Research/CCDPA_git/CCDPApy/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44833FB9-AF49-554D-9D81-AA3A71AF1344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B282EFB-F18D-004A-8C4B-B4DA3977C385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" activeTab="2" xr2:uid="{C7583198-B141-1C4B-B50F-A9FA90CFEBEA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{C7583198-B141-1C4B-B50F-A9FA90CFEBEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Measured Data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Ammonia</t>
+  </si>
+  <si>
+    <t>Bleeding Ratio, Beta</t>
   </si>
 </sst>
 </file>
@@ -662,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE2EEBC-76CD-9641-BDBB-B5D8CDAAE100}">
-  <dimension ref="A1:CO26"/>
+  <dimension ref="A1:CP26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -675,23 +678,24 @@
     <col min="3" max="3" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.1640625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="19.83203125" style="7" customWidth="1"/>
-    <col min="12" max="12" width="23.83203125" style="7" customWidth="1"/>
-    <col min="13" max="13" width="20.5" style="7" customWidth="1"/>
-    <col min="14" max="20" width="13.5" style="7" customWidth="1"/>
-    <col min="21" max="24" width="13.6640625" style="7" customWidth="1"/>
-    <col min="25" max="28" width="14" style="7" customWidth="1"/>
-    <col min="29" max="45" width="13.6640625" style="7" customWidth="1"/>
-    <col min="46" max="69" width="13.5" style="7" customWidth="1"/>
-    <col min="70" max="93" width="10.83203125" style="7"/>
-    <col min="94" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="15.83203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.1640625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="19.83203125" style="7" customWidth="1"/>
+    <col min="13" max="13" width="23.83203125" style="7" customWidth="1"/>
+    <col min="14" max="14" width="20.5" style="7" customWidth="1"/>
+    <col min="15" max="21" width="13.5" style="7" customWidth="1"/>
+    <col min="22" max="25" width="13.6640625" style="7" customWidth="1"/>
+    <col min="26" max="29" width="14" style="7" customWidth="1"/>
+    <col min="30" max="46" width="13.6640625" style="7" customWidth="1"/>
+    <col min="47" max="70" width="13.5" style="7" customWidth="1"/>
+    <col min="71" max="94" width="10.83203125" style="7"/>
+    <col min="95" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:93" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
@@ -703,13 +707,13 @@
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="9"/>
+      <c r="K1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="21"/>
       <c r="L1" s="21"/>
       <c r="M1" s="21"/>
-      <c r="N1" s="1"/>
+      <c r="N1" s="21"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -789,8 +793,9 @@
       <c r="CM1" s="1"/>
       <c r="CN1" s="1"/>
       <c r="CO1" s="1"/>
-    </row>
-    <row r="2" spans="1:93" ht="102" x14ac:dyDescent="0.2">
+      <c r="CP1" s="1"/>
+    </row>
+    <row r="2" spans="1:94" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
@@ -806,31 +811,33 @@
       <c r="E2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="K2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="35" t="s">
+      <c r="L2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="M2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="N2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -910,8 +917,9 @@
       <c r="CM2" s="1"/>
       <c r="CN2" s="1"/>
       <c r="CO2" s="1"/>
-    </row>
-    <row r="3" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="CP2" s="1"/>
+    </row>
+    <row r="3" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>43468</v>
       </c>
@@ -927,31 +935,33 @@
       <c r="E3" s="17">
         <v>500</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>0</v>
       </c>
       <c r="G3" s="18">
+        <v>0</v>
+      </c>
+      <c r="H3" s="18">
         <v>0.36212827761922883</v>
       </c>
-      <c r="H3" s="18">
+      <c r="I3" s="18">
         <v>0</v>
       </c>
-      <c r="I3" s="18">
+      <c r="J3" s="18">
         <v>0.362128277619229</v>
       </c>
-      <c r="J3" s="22">
+      <c r="K3" s="22">
         <v>3.459119496855346</v>
       </c>
-      <c r="K3" s="22">
+      <c r="L3" s="22">
         <v>0</v>
       </c>
-      <c r="L3" s="22">
+      <c r="M3" s="22">
         <v>6</v>
       </c>
-      <c r="M3" s="22">
+      <c r="N3" s="22">
         <v>0</v>
       </c>
-      <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -987,7 +997,7 @@
       <c r="AU3" s="3"/>
       <c r="AV3" s="3"/>
       <c r="AW3" s="3"/>
-      <c r="AX3" s="2"/>
+      <c r="AX3" s="3"/>
       <c r="AY3" s="2"/>
       <c r="AZ3" s="2"/>
       <c r="BA3" s="2"/>
@@ -1011,7 +1021,7 @@
       <c r="BS3" s="2"/>
       <c r="BT3" s="2"/>
       <c r="BU3" s="2"/>
-      <c r="BV3" s="1"/>
+      <c r="BV3" s="2"/>
       <c r="BW3" s="1"/>
       <c r="BX3" s="1"/>
       <c r="BY3" s="1"/>
@@ -1031,8 +1041,9 @@
       <c r="CM3" s="1"/>
       <c r="CN3" s="1"/>
       <c r="CO3" s="1"/>
-    </row>
-    <row r="4" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="CP3" s="1"/>
+    </row>
+    <row r="4" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <v>43468.416666666664</v>
       </c>
@@ -1048,31 +1059,33 @@
       <c r="E4" s="17">
         <v>500</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="17">
         <v>0</v>
       </c>
       <c r="G4" s="18">
+        <v>0</v>
+      </c>
+      <c r="H4" s="18">
         <v>0.56914052767871515</v>
       </c>
-      <c r="H4" s="18">
+      <c r="I4" s="18">
         <v>4.0997779370899212E-2</v>
       </c>
-      <c r="I4" s="18">
+      <c r="J4" s="18">
         <v>0.61013830704961436</v>
       </c>
-      <c r="J4" s="22">
+      <c r="K4" s="22">
         <v>3.1823899371069184</v>
       </c>
-      <c r="K4" s="22">
+      <c r="L4" s="22">
         <v>0.32704402515723269</v>
       </c>
-      <c r="L4" s="22">
+      <c r="M4" s="22">
         <v>5.8462613556953178</v>
       </c>
-      <c r="M4" s="22">
+      <c r="N4" s="22">
         <v>0.13081761006289308</v>
       </c>
-      <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -1108,7 +1121,7 @@
       <c r="AU4" s="3"/>
       <c r="AV4" s="3"/>
       <c r="AW4" s="3"/>
-      <c r="AX4" s="2"/>
+      <c r="AX4" s="3"/>
       <c r="AY4" s="2"/>
       <c r="AZ4" s="2"/>
       <c r="BA4" s="2"/>
@@ -1132,7 +1145,7 @@
       <c r="BS4" s="2"/>
       <c r="BT4" s="2"/>
       <c r="BU4" s="2"/>
-      <c r="BV4" s="1"/>
+      <c r="BV4" s="2"/>
       <c r="BW4" s="1"/>
       <c r="BX4" s="1"/>
       <c r="BY4" s="1"/>
@@ -1152,8 +1165,9 @@
       <c r="CM4" s="1"/>
       <c r="CN4" s="1"/>
       <c r="CO4" s="1"/>
-    </row>
-    <row r="5" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="CP4" s="1"/>
+    </row>
+    <row r="5" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
         <v>43468.833333333336</v>
       </c>
@@ -1169,31 +1183,33 @@
       <c r="E5" s="17">
         <v>500</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="17">
         <v>0</v>
       </c>
       <c r="G5" s="18">
+        <v>0</v>
+      </c>
+      <c r="H5" s="18">
         <v>0.98</v>
       </c>
-      <c r="H5" s="18">
+      <c r="I5" s="18">
         <v>1.2863981912312306E-2</v>
       </c>
-      <c r="I5" s="18">
+      <c r="J5" s="18">
         <v>0.99286398191231229</v>
       </c>
-      <c r="J5" s="22">
+      <c r="K5" s="22">
         <v>2.7169811320754715</v>
       </c>
-      <c r="K5" s="22">
+      <c r="L5" s="22">
         <v>0.80503144654088055</v>
       </c>
-      <c r="L5" s="22">
+      <c r="M5" s="22">
         <v>5.5877009084556253</v>
       </c>
-      <c r="M5" s="22">
+      <c r="N5" s="22">
         <v>0.32201257861635224</v>
       </c>
-      <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -1229,7 +1245,7 @@
       <c r="AU5" s="3"/>
       <c r="AV5" s="3"/>
       <c r="AW5" s="3"/>
-      <c r="AX5" s="2"/>
+      <c r="AX5" s="3"/>
       <c r="AY5" s="2"/>
       <c r="AZ5" s="2"/>
       <c r="BA5" s="2"/>
@@ -1253,7 +1269,7 @@
       <c r="BS5" s="2"/>
       <c r="BT5" s="2"/>
       <c r="BU5" s="2"/>
-      <c r="BV5" s="1"/>
+      <c r="BV5" s="2"/>
       <c r="BW5" s="1"/>
       <c r="BX5" s="1"/>
       <c r="BY5" s="1"/>
@@ -1273,8 +1289,9 @@
       <c r="CM5" s="1"/>
       <c r="CN5" s="1"/>
       <c r="CO5" s="1"/>
-    </row>
-    <row r="6" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="CP5" s="1"/>
+    </row>
+    <row r="6" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
         <v>43469.041666666664</v>
       </c>
@@ -1290,31 +1307,33 @@
       <c r="E6" s="17">
         <v>500</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="17">
         <v>0</v>
       </c>
       <c r="G6" s="18">
+        <v>0</v>
+      </c>
+      <c r="H6" s="18">
         <v>1.08</v>
       </c>
-      <c r="H6" s="18">
+      <c r="I6" s="18">
         <v>2.0000000000000018E-2</v>
       </c>
-      <c r="I6" s="18">
+      <c r="J6" s="18">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J6" s="22">
+      <c r="K6" s="22">
         <v>2.5</v>
       </c>
-      <c r="K6" s="22">
+      <c r="L6" s="22">
         <v>1</v>
       </c>
-      <c r="L6" s="22">
+      <c r="M6" s="22">
         <v>5.4671558350803631</v>
       </c>
-      <c r="M6" s="22">
+      <c r="N6" s="22">
         <v>0.4</v>
       </c>
-      <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -1350,7 +1369,7 @@
       <c r="AU6" s="3"/>
       <c r="AV6" s="3"/>
       <c r="AW6" s="3"/>
-      <c r="AX6" s="2"/>
+      <c r="AX6" s="3"/>
       <c r="AY6" s="2"/>
       <c r="AZ6" s="2"/>
       <c r="BA6" s="2"/>
@@ -1374,7 +1393,7 @@
       <c r="BS6" s="2"/>
       <c r="BT6" s="2"/>
       <c r="BU6" s="2"/>
-      <c r="BV6" s="1"/>
+      <c r="BV6" s="2"/>
       <c r="BW6" s="1"/>
       <c r="BX6" s="1"/>
       <c r="BY6" s="1"/>
@@ -1394,8 +1413,9 @@
       <c r="CM6" s="1"/>
       <c r="CN6" s="1"/>
       <c r="CO6" s="1"/>
-    </row>
-    <row r="7" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="CP6" s="1"/>
+    </row>
+    <row r="7" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <v>43469.25</v>
       </c>
@@ -1411,31 +1431,33 @@
       <c r="E7" s="17">
         <v>500</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="17">
+        <v>0</v>
+      </c>
+      <c r="G7" s="18">
         <v>5</v>
       </c>
-      <c r="G7" s="18">
+      <c r="H7" s="18">
         <v>1.4555865997453736</v>
       </c>
-      <c r="H7" s="18">
+      <c r="I7" s="18">
         <v>5.1514681416269026E-2</v>
       </c>
-      <c r="I7" s="18">
+      <c r="J7" s="18">
         <v>1.5071012811616427</v>
       </c>
-      <c r="J7" s="22">
+      <c r="K7" s="22">
         <v>2.2767295597484276</v>
       </c>
-      <c r="K7" s="22">
+      <c r="L7" s="22">
         <v>1.220125786163522</v>
       </c>
-      <c r="L7" s="22">
+      <c r="M7" s="22">
         <v>5.3431167016072676</v>
       </c>
-      <c r="M7" s="22">
+      <c r="N7" s="22">
         <v>0.48805031446540881</v>
       </c>
-      <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
@@ -1471,7 +1493,7 @@
       <c r="AU7" s="3"/>
       <c r="AV7" s="3"/>
       <c r="AW7" s="3"/>
-      <c r="AX7" s="2"/>
+      <c r="AX7" s="3"/>
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2"/>
       <c r="BA7" s="2"/>
@@ -1495,7 +1517,7 @@
       <c r="BS7" s="2"/>
       <c r="BT7" s="2"/>
       <c r="BU7" s="2"/>
-      <c r="BV7" s="1"/>
+      <c r="BV7" s="2"/>
       <c r="BW7" s="1"/>
       <c r="BX7" s="1"/>
       <c r="BY7" s="1"/>
@@ -1515,8 +1537,9 @@
       <c r="CM7" s="1"/>
       <c r="CN7" s="1"/>
       <c r="CO7" s="1"/>
-    </row>
-    <row r="8" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="CP7" s="1"/>
+    </row>
+    <row r="8" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
         <v>43469.458333333336</v>
       </c>
@@ -1532,31 +1555,33 @@
       <c r="E8" s="17">
         <v>500</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="17">
+        <v>0</v>
+      </c>
+      <c r="G8" s="18">
         <v>5</v>
       </c>
-      <c r="G8" s="18">
+      <c r="H8" s="18">
         <v>1.6156646373272472</v>
       </c>
-      <c r="H8" s="18">
+      <c r="I8" s="18">
         <v>0.17768260890764531</v>
       </c>
-      <c r="I8" s="18">
+      <c r="J8" s="18">
         <v>1.7933472462348925</v>
       </c>
-      <c r="J8" s="22">
+      <c r="K8" s="22">
         <v>1.9748427672955975</v>
       </c>
-      <c r="K8" s="22">
+      <c r="L8" s="22">
         <v>1.3459119496855345</v>
       </c>
-      <c r="L8" s="22">
+      <c r="M8" s="22">
         <v>5.1754018169112506</v>
       </c>
-      <c r="M8" s="22">
+      <c r="N8" s="22">
         <v>0.53836477987421383</v>
       </c>
-      <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -1592,7 +1617,7 @@
       <c r="AU8" s="3"/>
       <c r="AV8" s="3"/>
       <c r="AW8" s="3"/>
-      <c r="AX8" s="2"/>
+      <c r="AX8" s="3"/>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="2"/>
       <c r="BA8" s="2"/>
@@ -1616,7 +1641,7 @@
       <c r="BS8" s="2"/>
       <c r="BT8" s="2"/>
       <c r="BU8" s="2"/>
-      <c r="BV8" s="1"/>
+      <c r="BV8" s="2"/>
       <c r="BW8" s="1"/>
       <c r="BX8" s="1"/>
       <c r="BY8" s="1"/>
@@ -1636,8 +1661,9 @@
       <c r="CM8" s="1"/>
       <c r="CN8" s="1"/>
       <c r="CO8" s="1"/>
-    </row>
-    <row r="9" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="CP8" s="1"/>
+    </row>
+    <row r="9" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
         <v>43469.875</v>
       </c>
@@ -1653,31 +1679,33 @@
       <c r="E9" s="17">
         <v>500</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="17">
+        <v>0</v>
+      </c>
+      <c r="G9" s="18">
         <v>5</v>
       </c>
-      <c r="G9" s="18">
+      <c r="H9" s="18">
         <v>1.9905704880058399</v>
       </c>
-      <c r="H9" s="18">
+      <c r="I9" s="18">
         <v>0.37807198328859282</v>
       </c>
-      <c r="I9" s="18">
+      <c r="J9" s="18">
         <v>2.3686424712944327</v>
       </c>
-      <c r="J9" s="22">
+      <c r="K9" s="22">
         <v>1.4088050314465408</v>
       </c>
-      <c r="K9" s="22">
+      <c r="L9" s="22">
         <v>1.6855345911949686</v>
       </c>
-      <c r="L9" s="22">
+      <c r="M9" s="22">
         <v>4.8609364081062187</v>
       </c>
-      <c r="M9" s="22">
+      <c r="N9" s="22">
         <v>0.67421383647798749</v>
       </c>
-      <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
@@ -1713,7 +1741,7 @@
       <c r="AU9" s="3"/>
       <c r="AV9" s="3"/>
       <c r="AW9" s="3"/>
-      <c r="AX9" s="2"/>
+      <c r="AX9" s="3"/>
       <c r="AY9" s="2"/>
       <c r="AZ9" s="2"/>
       <c r="BA9" s="2"/>
@@ -1737,7 +1765,7 @@
       <c r="BS9" s="2"/>
       <c r="BT9" s="2"/>
       <c r="BU9" s="2"/>
-      <c r="BV9" s="1"/>
+      <c r="BV9" s="2"/>
       <c r="BW9" s="1"/>
       <c r="BX9" s="1"/>
       <c r="BY9" s="1"/>
@@ -1757,8 +1785,9 @@
       <c r="CM9" s="1"/>
       <c r="CN9" s="1"/>
       <c r="CO9" s="1"/>
-    </row>
-    <row r="10" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="CP9" s="1"/>
+    </row>
+    <row r="10" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
         <v>43470.5</v>
       </c>
@@ -1774,31 +1803,33 @@
       <c r="E10" s="17">
         <v>500</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="17">
+        <v>0</v>
+      </c>
+      <c r="G10" s="18">
         <v>10</v>
       </c>
-      <c r="G10" s="18">
+      <c r="H10" s="18">
         <v>3.0215531909396138</v>
       </c>
-      <c r="H10" s="18">
+      <c r="I10" s="18">
         <v>0.57388804586113373</v>
       </c>
-      <c r="I10" s="18">
+      <c r="J10" s="18">
         <v>3.5954412368007476</v>
       </c>
-      <c r="J10" s="22">
+      <c r="K10" s="22">
         <v>0.90566037735849059</v>
       </c>
-      <c r="K10" s="22">
+      <c r="L10" s="22">
         <v>2.1886792452830188</v>
       </c>
-      <c r="L10" s="22">
+      <c r="M10" s="22">
         <v>4.581411600279524</v>
       </c>
-      <c r="M10" s="22">
+      <c r="N10" s="22">
         <v>0.87547169811320757</v>
       </c>
-      <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
@@ -1834,7 +1865,7 @@
       <c r="AU10" s="3"/>
       <c r="AV10" s="3"/>
       <c r="AW10" s="3"/>
-      <c r="AX10" s="2"/>
+      <c r="AX10" s="3"/>
       <c r="AY10" s="2"/>
       <c r="AZ10" s="2"/>
       <c r="BA10" s="2"/>
@@ -1858,7 +1889,7 @@
       <c r="BS10" s="2"/>
       <c r="BT10" s="2"/>
       <c r="BU10" s="2"/>
-      <c r="BV10" s="1"/>
+      <c r="BV10" s="2"/>
       <c r="BW10" s="1"/>
       <c r="BX10" s="1"/>
       <c r="BY10" s="1"/>
@@ -1878,8 +1909,9 @@
       <c r="CM10" s="1"/>
       <c r="CN10" s="1"/>
       <c r="CO10" s="1"/>
-    </row>
-    <row r="11" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="CP10" s="1"/>
+    </row>
+    <row r="11" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
         <v>43470.916666666664</v>
       </c>
@@ -1895,31 +1927,33 @@
       <c r="E11" s="17">
         <v>500</v>
       </c>
-      <c r="F11" s="18">
-        <v>15</v>
+      <c r="F11" s="17">
+        <v>0</v>
       </c>
       <c r="G11" s="18">
+        <v>15</v>
+      </c>
+      <c r="H11" s="18">
         <v>3.7226875372936807</v>
       </c>
-      <c r="H11" s="18">
+      <c r="I11" s="18">
         <v>0.70705552446843933</v>
       </c>
-      <c r="I11" s="18">
+      <c r="J11" s="18">
         <v>4.4297430617621201</v>
       </c>
-      <c r="J11" s="22">
+      <c r="K11" s="22">
         <v>0.88050314465408808</v>
       </c>
-      <c r="K11" s="22">
+      <c r="L11" s="22">
         <v>2.2389937106918238</v>
       </c>
-      <c r="L11" s="22">
+      <c r="M11" s="22">
         <v>4.5674353598881892</v>
       </c>
-      <c r="M11" s="22">
+      <c r="N11" s="22">
         <v>0.89559748427672958</v>
       </c>
-      <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
@@ -1955,7 +1989,7 @@
       <c r="AU11" s="3"/>
       <c r="AV11" s="3"/>
       <c r="AW11" s="3"/>
-      <c r="AX11" s="2"/>
+      <c r="AX11" s="3"/>
       <c r="AY11" s="2"/>
       <c r="AZ11" s="2"/>
       <c r="BA11" s="2"/>
@@ -1979,7 +2013,7 @@
       <c r="BS11" s="2"/>
       <c r="BT11" s="2"/>
       <c r="BU11" s="2"/>
-      <c r="BV11" s="1"/>
+      <c r="BV11" s="2"/>
       <c r="BW11" s="1"/>
       <c r="BX11" s="1"/>
       <c r="BY11" s="1"/>
@@ -1999,8 +2033,9 @@
       <c r="CM11" s="1"/>
       <c r="CN11" s="1"/>
       <c r="CO11" s="1"/>
-    </row>
-    <row r="12" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="CP11" s="1"/>
+    </row>
+    <row r="12" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <v>43471.333333333336</v>
       </c>
@@ -2016,31 +2051,33 @@
       <c r="E12" s="17">
         <v>500</v>
       </c>
-      <c r="F12" s="18">
-        <v>15</v>
+      <c r="F12" s="17">
+        <v>0</v>
       </c>
       <c r="G12" s="18">
+        <v>15</v>
+      </c>
+      <c r="H12" s="18">
         <v>5.090917949574572</v>
       </c>
-      <c r="H12" s="18">
+      <c r="I12" s="18">
         <v>0.9669255409705988</v>
       </c>
-      <c r="I12" s="18">
+      <c r="J12" s="18">
         <v>6.0578434905451708</v>
       </c>
-      <c r="J12" s="22">
+      <c r="K12" s="22">
         <v>0.76729559748427678</v>
       </c>
-      <c r="K12" s="22">
+      <c r="L12" s="22">
         <v>2.3773584905660377</v>
       </c>
-      <c r="L12" s="22">
+      <c r="M12" s="22">
         <v>4.5045422781271824</v>
       </c>
-      <c r="M12" s="22">
+      <c r="N12" s="22">
         <v>0.95094339622641511</v>
       </c>
-      <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -2076,7 +2113,7 @@
       <c r="AU12" s="3"/>
       <c r="AV12" s="3"/>
       <c r="AW12" s="3"/>
-      <c r="AX12" s="2"/>
+      <c r="AX12" s="3"/>
       <c r="AY12" s="2"/>
       <c r="AZ12" s="2"/>
       <c r="BA12" s="2"/>
@@ -2100,7 +2137,7 @@
       <c r="BS12" s="2"/>
       <c r="BT12" s="2"/>
       <c r="BU12" s="2"/>
-      <c r="BV12" s="1"/>
+      <c r="BV12" s="2"/>
       <c r="BW12" s="1"/>
       <c r="BX12" s="1"/>
       <c r="BY12" s="1"/>
@@ -2120,8 +2157,9 @@
       <c r="CM12" s="1"/>
       <c r="CN12" s="1"/>
       <c r="CO12" s="1"/>
-    </row>
-    <row r="13" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="CP12" s="1"/>
+    </row>
+    <row r="13" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A13" s="15">
         <v>43471.75</v>
       </c>
@@ -2137,31 +2175,33 @@
       <c r="E13" s="17">
         <v>500</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="17">
+        <v>0</v>
+      </c>
+      <c r="G13" s="18">
         <v>20</v>
       </c>
-      <c r="G13" s="18">
+      <c r="H13" s="18">
         <v>6.2722366963768454</v>
       </c>
-      <c r="H13" s="18">
+      <c r="I13" s="18">
         <v>1.1912951496785809</v>
       </c>
-      <c r="I13" s="18">
+      <c r="J13" s="18">
         <v>7.4635318460554263</v>
       </c>
-      <c r="J13" s="22">
+      <c r="K13" s="22">
         <v>0.64150943396226412</v>
       </c>
-      <c r="K13" s="22">
+      <c r="L13" s="22">
         <v>2.3270440251572326</v>
       </c>
-      <c r="L13" s="22">
+      <c r="M13" s="22">
         <v>4.4346610761705083</v>
       </c>
-      <c r="M13" s="22">
+      <c r="N13" s="22">
         <v>0.9308176100628931</v>
       </c>
-      <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
@@ -2197,7 +2237,7 @@
       <c r="AU13" s="3"/>
       <c r="AV13" s="3"/>
       <c r="AW13" s="3"/>
-      <c r="AX13" s="2"/>
+      <c r="AX13" s="3"/>
       <c r="AY13" s="2"/>
       <c r="AZ13" s="2"/>
       <c r="BA13" s="2"/>
@@ -2221,7 +2261,7 @@
       <c r="BS13" s="2"/>
       <c r="BT13" s="2"/>
       <c r="BU13" s="2"/>
-      <c r="BV13" s="1"/>
+      <c r="BV13" s="2"/>
       <c r="BW13" s="1"/>
       <c r="BX13" s="1"/>
       <c r="BY13" s="1"/>
@@ -2241,8 +2281,9 @@
       <c r="CM13" s="1"/>
       <c r="CN13" s="1"/>
       <c r="CO13" s="1"/>
-    </row>
-    <row r="14" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="CP13" s="1"/>
+    </row>
+    <row r="14" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A14" s="15">
         <v>43471.958333333336</v>
       </c>
@@ -2258,31 +2299,33 @@
       <c r="E14" s="17">
         <v>500</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="17">
+        <v>0</v>
+      </c>
+      <c r="G14" s="18">
         <v>25</v>
       </c>
-      <c r="G14" s="18">
+      <c r="H14" s="18">
         <v>6.7935460000000001</v>
       </c>
-      <c r="H14" s="18">
+      <c r="I14" s="18">
         <v>1.7210410000000005</v>
       </c>
-      <c r="I14" s="18">
+      <c r="J14" s="18">
         <v>8.5145870000000006</v>
       </c>
-      <c r="J14" s="22">
+      <c r="K14" s="22">
         <v>0.66</v>
       </c>
-      <c r="K14" s="22">
+      <c r="L14" s="22">
         <v>2.4700000000000002</v>
       </c>
-      <c r="L14" s="22">
+      <c r="M14" s="22">
         <v>4.4449336128581391</v>
       </c>
-      <c r="M14" s="22">
+      <c r="N14" s="22">
         <v>0.9880000000000001</v>
       </c>
-      <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
@@ -2318,7 +2361,7 @@
       <c r="AU14" s="3"/>
       <c r="AV14" s="3"/>
       <c r="AW14" s="3"/>
-      <c r="AX14" s="2"/>
+      <c r="AX14" s="3"/>
       <c r="AY14" s="2"/>
       <c r="AZ14" s="2"/>
       <c r="BA14" s="2"/>
@@ -2342,7 +2385,7 @@
       <c r="BS14" s="2"/>
       <c r="BT14" s="2"/>
       <c r="BU14" s="2"/>
-      <c r="BV14" s="1"/>
+      <c r="BV14" s="2"/>
       <c r="BW14" s="1"/>
       <c r="BX14" s="1"/>
       <c r="BY14" s="1"/>
@@ -2362,8 +2405,9 @@
       <c r="CM14" s="1"/>
       <c r="CN14" s="1"/>
       <c r="CO14" s="1"/>
-    </row>
-    <row r="15" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="CP14" s="1"/>
+    </row>
+    <row r="15" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
         <v>43472.166666666664</v>
       </c>
@@ -2379,31 +2423,33 @@
       <c r="E15" s="17">
         <v>500</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="17">
+        <v>0</v>
+      </c>
+      <c r="G15" s="18">
         <v>30</v>
       </c>
-      <c r="G15" s="18">
+      <c r="H15" s="18">
         <v>7.2084186230122125</v>
       </c>
-      <c r="H15" s="18">
+      <c r="I15" s="18">
         <v>2.312418201637005</v>
       </c>
-      <c r="I15" s="18">
+      <c r="J15" s="18">
         <v>9.5208368246492174</v>
       </c>
-      <c r="J15" s="22">
+      <c r="K15" s="22">
         <v>0.75471698113207553</v>
       </c>
-      <c r="K15" s="22">
+      <c r="L15" s="22">
         <v>2.3647798742138364</v>
       </c>
-      <c r="L15" s="22">
+      <c r="M15" s="22">
         <v>4.4975541579315141</v>
       </c>
-      <c r="M15" s="22">
+      <c r="N15" s="22">
         <v>0.9459119496855346</v>
       </c>
-      <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
@@ -2439,7 +2485,7 @@
       <c r="AU15" s="3"/>
       <c r="AV15" s="3"/>
       <c r="AW15" s="3"/>
-      <c r="AX15" s="2"/>
+      <c r="AX15" s="3"/>
       <c r="AY15" s="2"/>
       <c r="AZ15" s="2"/>
       <c r="BA15" s="2"/>
@@ -2463,7 +2509,7 @@
       <c r="BS15" s="2"/>
       <c r="BT15" s="2"/>
       <c r="BU15" s="2"/>
-      <c r="BV15" s="1"/>
+      <c r="BV15" s="2"/>
       <c r="BW15" s="1"/>
       <c r="BX15" s="1"/>
       <c r="BY15" s="1"/>
@@ -2483,8 +2529,9 @@
       <c r="CM15" s="1"/>
       <c r="CN15" s="1"/>
       <c r="CO15" s="1"/>
-    </row>
-    <row r="16" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="CP15" s="1"/>
+    </row>
+    <row r="16" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A16" s="15">
         <v>43472.791666666664</v>
       </c>
@@ -2500,31 +2547,33 @@
       <c r="E16" s="17">
         <v>500</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="17">
+        <v>0</v>
+      </c>
+      <c r="G16" s="19">
         <v>35</v>
       </c>
-      <c r="G16" s="19">
+      <c r="H16" s="19">
         <v>8.577524184256049</v>
       </c>
-      <c r="H16" s="19">
+      <c r="I16" s="19">
         <v>1.9903660244334311</v>
       </c>
-      <c r="I16" s="19">
+      <c r="J16" s="19">
         <v>10.56789020868948</v>
       </c>
-      <c r="J16" s="23">
+      <c r="K16" s="23">
         <v>0.8176100628930818</v>
       </c>
-      <c r="K16" s="23">
+      <c r="L16" s="23">
         <v>2.3018867924528301</v>
       </c>
-      <c r="L16" s="23">
+      <c r="M16" s="23">
         <v>4.5324947589098512</v>
       </c>
-      <c r="M16" s="23">
+      <c r="N16" s="23">
         <v>0.92075471698113209</v>
       </c>
-      <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
@@ -2532,7 +2581,7 @@
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
       <c r="U16" s="5"/>
-      <c r="V16" s="6"/>
+      <c r="V16" s="5"/>
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
       <c r="Y16" s="6"/>
@@ -2556,8 +2605,9 @@
       <c r="AQ16" s="6"/>
       <c r="AR16" s="6"/>
       <c r="AS16" s="6"/>
-    </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT16" s="6"/>
+    </row>
+    <row r="17" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A17" s="15">
         <v>43473.208333333336</v>
       </c>
@@ -2573,31 +2623,33 @@
       <c r="E17" s="17">
         <v>500</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="19">
         <v>35</v>
       </c>
-      <c r="G17" s="19">
+      <c r="H17" s="19">
         <v>9.8577888657877395</v>
       </c>
-      <c r="H17" s="19">
+      <c r="I17" s="19">
         <v>2.2874442103602934</v>
       </c>
-      <c r="I17" s="19">
+      <c r="J17" s="19">
         <v>12.145233076148033</v>
       </c>
-      <c r="J17" s="23">
+      <c r="K17" s="23">
         <v>0.80503144654088055</v>
       </c>
-      <c r="K17" s="23">
+      <c r="L17" s="23">
         <v>2.2012578616352201</v>
       </c>
-      <c r="L17" s="23">
+      <c r="M17" s="23">
         <v>4.5255066387141838</v>
       </c>
-      <c r="M17" s="23">
+      <c r="N17" s="23">
         <v>0.88050314465408808</v>
       </c>
-      <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
@@ -2605,7 +2657,7 @@
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
       <c r="U17" s="5"/>
-      <c r="V17" s="6"/>
+      <c r="V17" s="5"/>
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
       <c r="Y17" s="6"/>
@@ -2629,8 +2681,9 @@
       <c r="AQ17" s="6"/>
       <c r="AR17" s="6"/>
       <c r="AS17" s="6"/>
-    </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT17" s="6"/>
+    </row>
+    <row r="18" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A18" s="20">
         <v>43473.833333333336</v>
       </c>
@@ -2646,32 +2699,35 @@
       <c r="E18" s="17">
         <v>500</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="17">
+        <v>0</v>
+      </c>
+      <c r="G18" s="19">
         <v>35</v>
       </c>
-      <c r="G18" s="19">
+      <c r="H18" s="19">
         <v>10.94189852769845</v>
       </c>
-      <c r="H18" s="19">
+      <c r="I18" s="19">
         <v>2.5390057322488175</v>
       </c>
-      <c r="I18" s="19">
+      <c r="J18" s="19">
         <v>13.480904259947268</v>
       </c>
-      <c r="J18" s="24">
+      <c r="K18" s="24">
         <v>0.70440251572327039</v>
       </c>
-      <c r="K18" s="24">
+      <c r="L18" s="24">
         <v>2.1635220125786163</v>
       </c>
-      <c r="L18" s="24">
+      <c r="M18" s="24">
         <v>4.4696016771488445</v>
       </c>
-      <c r="M18" s="24">
+      <c r="N18" s="24">
         <v>0.86540880503144657</v>
       </c>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A19" s="20">
         <v>43474.25</v>
       </c>
@@ -2687,32 +2743,35 @@
       <c r="E19" s="17">
         <v>500</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="G19" s="19">
         <v>40</v>
       </c>
-      <c r="G19" s="19">
+      <c r="H19" s="19">
         <v>12.57506515398768</v>
       </c>
-      <c r="H19" s="19">
+      <c r="I19" s="19">
         <v>2.9179728205808484</v>
       </c>
-      <c r="I19" s="19">
+      <c r="J19" s="19">
         <v>15.493037974568528</v>
       </c>
-      <c r="J19" s="24">
+      <c r="K19" s="24">
         <v>0.70440251572327039</v>
       </c>
-      <c r="K19" s="24">
+      <c r="L19" s="24">
         <v>2.2893081761006289</v>
       </c>
-      <c r="L19" s="24">
+      <c r="M19" s="24">
         <v>4.4696016771488445</v>
       </c>
-      <c r="M19" s="24">
+      <c r="N19" s="24">
         <v>0.91572327044025159</v>
       </c>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A20" s="20">
         <v>43474.666666666664</v>
       </c>
@@ -2728,32 +2787,35 @@
       <c r="E20" s="17">
         <v>500</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="G20" s="19">
         <v>40</v>
       </c>
-      <c r="G20" s="19">
+      <c r="H20" s="19">
         <v>11.329143379253193</v>
       </c>
-      <c r="H20" s="19">
+      <c r="I20" s="19">
         <v>2.6288637121407845</v>
       </c>
-      <c r="I20" s="19">
+      <c r="J20" s="19">
         <v>13.958007091393977</v>
       </c>
-      <c r="J20" s="24">
+      <c r="K20" s="24">
         <v>0.80503144654088055</v>
       </c>
-      <c r="K20" s="24">
+      <c r="L20" s="24">
         <v>2.4150943396226414</v>
       </c>
-      <c r="L20" s="24">
+      <c r="M20" s="24">
         <v>4.5255066387141838</v>
       </c>
-      <c r="M20" s="24">
+      <c r="N20" s="24">
         <v>0.96603773584905661</v>
       </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A21" s="20">
         <v>43475.291666666664</v>
       </c>
@@ -2769,32 +2831,35 @@
       <c r="E21" s="17">
         <v>500</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="17">
+        <v>0</v>
+      </c>
+      <c r="G21" s="19">
         <v>40</v>
       </c>
-      <c r="G21" s="19">
+      <c r="H21" s="19">
         <v>10.56789020868948</v>
       </c>
-      <c r="H21" s="19">
+      <c r="I21" s="19">
         <v>2.9130140512577878</v>
       </c>
-      <c r="I21" s="19">
+      <c r="J21" s="19">
         <v>13.480904259947268</v>
       </c>
-      <c r="J21" s="24">
+      <c r="K21" s="24">
         <v>0.74213836477987416</v>
       </c>
-      <c r="K21" s="24">
+      <c r="L21" s="24">
         <v>2.3522012578616351</v>
       </c>
-      <c r="L21" s="24">
+      <c r="M21" s="24">
         <v>4.4905660377358467</v>
       </c>
-      <c r="M21" s="24">
+      <c r="N21" s="24">
         <v>0.9408805031446541</v>
       </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A22" s="20">
         <v>43475.916666666664</v>
       </c>
@@ -2810,32 +2875,35 @@
       <c r="E22" s="17">
         <v>500</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="17">
+        <v>0</v>
+      </c>
+      <c r="G22" s="19">
         <v>40</v>
       </c>
-      <c r="G22" s="19">
+      <c r="H22" s="19">
         <v>10.94189852769845</v>
       </c>
-      <c r="H22" s="19">
+      <c r="I22" s="19">
         <v>3.510096546715495</v>
       </c>
-      <c r="I22" s="19">
+      <c r="J22" s="19">
         <v>14.451995074413945</v>
       </c>
-      <c r="J22" s="24">
+      <c r="K22" s="24">
         <v>0.83018867924528306</v>
       </c>
-      <c r="K22" s="24">
+      <c r="L22" s="24">
         <v>2.2515723270440251</v>
       </c>
-      <c r="L22" s="24">
+      <c r="M22" s="24">
         <v>4.5394828791055186</v>
       </c>
-      <c r="M22" s="24">
+      <c r="N22" s="24">
         <v>0.90062893081761008</v>
       </c>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A23" s="20">
         <v>43476.333333333336</v>
       </c>
@@ -2851,32 +2919,35 @@
       <c r="E23" s="17">
         <v>500</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="17">
+        <v>0</v>
+      </c>
+      <c r="G23" s="19">
         <v>40</v>
       </c>
-      <c r="G23" s="19">
+      <c r="H23" s="19">
         <v>9.8577888657877395</v>
       </c>
-      <c r="H23" s="19">
+      <c r="I23" s="19">
         <v>3.6231153941595284</v>
       </c>
-      <c r="I23" s="19">
+      <c r="J23" s="19">
         <v>13.480904259947268</v>
       </c>
-      <c r="J23" s="24">
+      <c r="K23" s="24">
         <v>0.70440251572327039</v>
       </c>
-      <c r="K23" s="24">
+      <c r="L23" s="24">
         <v>2.3522012578616351</v>
       </c>
-      <c r="L23" s="24">
+      <c r="M23" s="24">
         <v>4.4696016771488445</v>
       </c>
-      <c r="M23" s="24">
+      <c r="N23" s="24">
         <v>0.9408805031446541</v>
       </c>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A24" s="20">
         <v>43476.75</v>
       </c>
@@ -2892,32 +2963,35 @@
       <c r="E24" s="17">
         <v>500</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="17">
+        <v>0</v>
+      </c>
+      <c r="G24" s="19">
         <v>40</v>
       </c>
-      <c r="G24" s="19">
+      <c r="H24" s="19">
         <v>9.8577888657877395</v>
       </c>
-      <c r="H24" s="19">
+      <c r="I24" s="19">
         <v>4.5942062086262059</v>
       </c>
-      <c r="I24" s="19">
+      <c r="J24" s="19">
         <v>14.451995074413945</v>
       </c>
-      <c r="J24" s="24">
+      <c r="K24" s="24">
         <v>0.67924528301886788</v>
       </c>
-      <c r="K24" s="24">
+      <c r="L24" s="24">
         <v>2.4779874213836477</v>
       </c>
-      <c r="L24" s="24">
+      <c r="M24" s="24">
         <v>4.4556254367575097</v>
       </c>
-      <c r="M24" s="24">
+      <c r="N24" s="24">
         <v>0.99119496855345912</v>
       </c>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A25" s="20">
         <v>43477.166666666664</v>
       </c>
@@ -2933,32 +3007,35 @@
       <c r="E25" s="17">
         <v>500</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="17">
+        <v>0</v>
+      </c>
+      <c r="G25" s="19">
         <v>40</v>
       </c>
-      <c r="G25" s="19">
+      <c r="H25" s="19">
         <v>10.206665980332991</v>
       </c>
-      <c r="H25" s="19">
+      <c r="I25" s="19">
         <v>5.2863719942355374</v>
       </c>
-      <c r="I25" s="19">
+      <c r="J25" s="19">
         <v>15.493037974568528</v>
       </c>
-      <c r="J25" s="24">
+      <c r="K25" s="24">
         <v>0.75471698113207553</v>
       </c>
-      <c r="K25" s="24">
+      <c r="L25" s="24">
         <v>2.5157232704402515</v>
       </c>
-      <c r="L25" s="24">
+      <c r="M25" s="24">
         <v>4.4975541579315141</v>
       </c>
-      <c r="M25" s="24">
+      <c r="N25" s="24">
         <v>1.0062893081761006</v>
       </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A26" s="20">
         <v>43477.583333333336</v>
       </c>
@@ -2974,28 +3051,31 @@
       <c r="E26" s="17">
         <v>500</v>
       </c>
-      <c r="F26" s="19">
+      <c r="F26" s="17">
+        <v>0</v>
+      </c>
+      <c r="G26" s="19">
         <v>40</v>
       </c>
-      <c r="G26" s="19">
+      <c r="H26" s="19">
         <v>9.8577888657877395</v>
       </c>
-      <c r="H26" s="19">
+      <c r="I26" s="19">
         <v>4.1002182256062376</v>
       </c>
-      <c r="I26" s="19">
+      <c r="J26" s="19">
         <v>13.958007091393977</v>
       </c>
-      <c r="J26" s="24">
+      <c r="K26" s="24">
         <v>0.80503144654088055</v>
       </c>
-      <c r="K26" s="24">
+      <c r="L26" s="24">
         <v>2.5031446540880502</v>
       </c>
-      <c r="L26" s="24">
+      <c r="M26" s="24">
         <v>4.5255066387141838</v>
       </c>
-      <c r="M26" s="24">
+      <c r="N26" s="24">
         <v>1.0012578616352201</v>
       </c>
     </row>
@@ -3509,7 +3589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27B839A-4138-1B42-BC7A-A5BF803D2EB7}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>